<commit_message>
UI changes and method implementation
Implemented stop, previous, next methods and some UI changes.
</commit_message>
<xml_diff>
--- a/docs/exercise/GradedExercise.xlsx
+++ b/docs/exercise/GradedExercise.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samto\Documents\Dropbox\01 FHNW\01 Unterricht\08 8. Semester, FS 17\02_4iCbb_webeC\vscode_workspace\bewertete-uebung-stokalakis\docs\exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\01_FHNW\01_Unterricht\08_8_Semester_FS17\02_4iCbb_webeC\vscode_workspace\bewertete-uebung-stokalakis\docs\exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="1776" windowWidth="18660" windowHeight="17664" tabRatio="500"/>
+    <workbookView xWindow="7380" yWindow="1770" windowWidth="18660" windowHeight="17670" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -599,22 +599,22 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.796875" customWidth="1"/>
-    <col min="3" max="3" width="14.69921875" customWidth="1"/>
-    <col min="4" max="4" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.296875" customWidth="1"/>
+    <col min="1" max="1" width="5.75" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -637,7 +637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>5</v>
       </c>
@@ -645,10 +645,10 @@
         <v>6</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>15</v>
       </c>
@@ -656,10 +656,10 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -668,14 +668,14 @@
       </c>
       <c r="G6" s="4">
         <f>SUM(G4:G5)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H6" s="4">
         <f>MIN(C6,G6)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>2</v>
       </c>
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>2</v>
       </c>
@@ -697,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>3</v>
       </c>
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>5</v>
       </c>
@@ -716,10 +716,10 @@
         <v>7</v>
       </c>
       <c r="G11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>10</v>
       </c>
@@ -727,10 +727,10 @@
         <v>4</v>
       </c>
       <c r="G12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -739,18 +739,18 @@
       </c>
       <c r="G13" s="4">
         <f>SUM(G8:G12)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H13" s="4">
         <f>MIN(C13,G13)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>5</v>
       </c>
@@ -761,7 +761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>5</v>
       </c>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>2</v>
       </c>
@@ -783,7 +783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>2</v>
       </c>
@@ -791,10 +791,10 @@
         <v>11</v>
       </c>
       <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>2</v>
       </c>
@@ -802,10 +802,10 @@
         <v>14</v>
       </c>
       <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>2</v>
       </c>
@@ -816,7 +816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>2</v>
       </c>
@@ -824,10 +824,10 @@
         <v>16</v>
       </c>
       <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
@@ -836,14 +836,14 @@
       </c>
       <c r="G22" s="4">
         <f>SUM(G15:G21)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H22" s="4">
         <f>MIN(C22,G22)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>5</v>
       </c>
@@ -854,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>5</v>
       </c>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>5</v>
       </c>
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>5</v>
       </c>
@@ -887,7 +887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>5</v>
       </c>
@@ -898,7 +898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
@@ -914,7 +914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>25</v>
       </c>
@@ -923,14 +923,14 @@
       </c>
       <c r="H32">
         <f>SUM(H4:H29)</f>
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I32">
         <f>MIN(C32,H32)</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>30</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="6">
         <f>1 + TOTAL_POINTS/10</f>
-        <v>4.4000000000000004</v>
+        <v>5.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>